<commit_message>
menambahkan model 2 dan 3
</commit_message>
<xml_diff>
--- a/sprint_project.xlsx
+++ b/sprint_project.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dokumen Penting\TB_Praktikum\TugasPraktikumML_212-202\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07347C0B-C98D-4A0E-9ACF-DCF3E32D39F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA116C7-443E-4578-B907-D1B41786BD31}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580" xr2:uid="{69785BDA-A4B7-4DF2-AA12-13B89B42EC3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Lembar1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="33">
   <si>
     <t>Sprint Project</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Save Model 1 dan 2</t>
   </si>
   <si>
-    <t>Development Front-End Web</t>
-  </si>
-  <si>
     <t>Configurasi Flask</t>
   </si>
   <si>
@@ -109,6 +106,24 @@
   </si>
   <si>
     <t>26 Oktober</t>
+  </si>
+  <si>
+    <t>Membuat image generator</t>
+  </si>
+  <si>
+    <t>8 Nopember</t>
+  </si>
+  <si>
+    <t>Testing Model 1</t>
+  </si>
+  <si>
+    <t>Testing Model 2</t>
+  </si>
+  <si>
+    <t>Testing Model 3</t>
+  </si>
+  <si>
+    <t>9 Nopember</t>
   </si>
 </sst>
 </file>
@@ -684,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BCF303D-17AF-4351-B443-16E0FF75AF1B}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -748,16 +763,16 @@
         <v>10</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -768,16 +783,16 @@
         <v>11</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -788,16 +803,16 @@
         <v>12</v>
       </c>
       <c r="C6" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="13" t="s">
         <v>24</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>25</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>8</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -808,16 +823,16 @@
         <v>13</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>8</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -828,16 +843,16 @@
         <v>14</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>9</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -848,16 +863,16 @@
         <v>15</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -868,32 +883,36 @@
         <v>16</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>9</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
         <v>8</v>
       </c>
-      <c r="B11" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
+      <c r="B11" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>28</v>
+      </c>
       <c r="E11" s="15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
@@ -901,49 +920,111 @@
         <v>9</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
+        <v>29</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>28</v>
+      </c>
       <c r="E12" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="F12" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <v>10</v>
       </c>
       <c r="B13" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="12">
+        <v>11</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="12">
+        <v>12</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="12">
+        <v>13</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="20">
+        <v>14</v>
+      </c>
+      <c r="B17" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="14" t="s">
+      <c r="C17" s="21"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="16" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="20"/>
-      <c r="B14" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C19" s="4"/>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C22" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>